<commit_message>
Fixed update_quest.pu not iterating through quest titles from quest_titles.xlsx
</commit_message>
<xml_diff>
--- a/quest_data.xlsx
+++ b/quest_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -28,10 +28,118 @@
     <t xml:space="preserve">QuestType</t>
   </si>
   <si>
-    <t xml:space="preserve">01_Farm4_BuildWorkbench</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Build</t>
+    <t xml:space="preserve">89_Farm4_RemoveTree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BuildDecor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90_Farm4_ClearLaboratorySpace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91_Farm4_CollectAloe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">92_Farm4_BuildLaboratory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BuildWorkshop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">93_Farm4_StartCraftReagent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartCraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94_Farm4_ClearMapPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95_Farm4_BuildMap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96_Farm4_ClearLibraryPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97_Farm4_BuildLibrary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98_Farm4_ClearBridgePath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99_Farm4_BuildBridgeZF5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100_Farm4_FindLabNotes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101_Farm4_ClearDoghouseSpace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">102_Farm4_BuildDoghoulse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">103_Farm4_BuildDogPark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">104_Farm4_CollectOpunita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">105_Farm4_StartCrafJam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">106_Farm4_ClearPoundSpace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">107_Farm4_BuildPound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">108_Farm4_ClearMountainPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109_Farm4_CollectClay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110_Farm4_StartCraftSprayer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111_Farm4_ClearBlockerZF6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">112_Farm4_CollectCoal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">113_Farm4_StartCraftResperator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">114_Farm4_CollectEdelweiss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">115_Farm4_ClearDomeSpace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">116_Farm4_BuildDome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">117_Farm4_CleanTrainingCamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">118_Farm4_BuildTrainingCamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">119_Farm4_BuildSuitsCloset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120_Farm4_StartCraftBiohazardSuit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">121_Farm4_SprayAntidote</t>
   </si>
 </sst>
 </file>
@@ -113,7 +221,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -130,12 +238,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -155,10 +271,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -184,7 +300,275 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Update _Close atribute script added
</commit_message>
<xml_diff>
--- a/quest_data.xlsx
+++ b/quest_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t xml:space="preserve">NameXml</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">ParentQuest</t>
   </si>
   <si>
+    <t xml:space="preserve">CloseQuest</t>
+  </si>
+  <si>
     <t xml:space="preserve">89_Farm4_RemoveTree.xml</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t xml:space="preserve">88_Farm4_BuildFerrisWheel</t>
   </si>
   <si>
+    <t xml:space="preserve">Farm4_RemoveTree_Close</t>
+  </si>
+  <si>
     <t xml:space="preserve">90_Farm4_ClearLaboratorySpace.xml</t>
   </si>
   <si>
@@ -64,6 +70,9 @@
     <t xml:space="preserve">Farm4_quest90</t>
   </si>
   <si>
+    <t xml:space="preserve">Farm4_ClearLaboratorySpace_Close</t>
+  </si>
+  <si>
     <t xml:space="preserve">91_Farm4_CollectAloe.xml</t>
   </si>
   <si>
@@ -74,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">Farm4_quest91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farm4_CollectAloe_Close</t>
   </si>
 </sst>
 </file>
@@ -155,21 +167,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -180,12 +188,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -209,209 +217,221 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="37.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="30.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="9.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="13.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="29.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="31.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>6</v>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>11</v>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>